<commit_message>
add driver xls file chage
</commit_message>
<xml_diff>
--- a/public/sample/driver_bulkimport.xlsx
+++ b/public/sample/driver_bulkimport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FR-CHD-00471\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\easemylr-pro\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED184D6-57A8-4422-A250-D05824008A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A8CD3-C2D8-4709-94A0-F8AF72D55555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CE7AA421-B762-42AB-8B03-FBDBD462F790}"/>
   </bookViews>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t>deepak</t>
-  </si>
-  <si>
-    <t>deepak@yopmail.com</t>
   </si>
   <si>
     <t>lincno8938744</t>
@@ -65,24 +59,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,16 +85,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,20 +404,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F36C267-5877-40F1-9E62-9D7F6D695E7D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,29 +430,20 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>9867687678</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>9867687678</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{1F10CF97-9E94-4B22-AFAD-79C418D1AA84}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>